<commit_message>
started IRF type analysis
</commit_message>
<xml_diff>
--- a/workingfolder/OtherData/InfShocks.xlsx
+++ b/workingfolder/OtherData/InfShocks.xlsx
@@ -14,7 +14,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="68" uniqueCount="15">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="9" uniqueCount="9">
   <si>
     <t>pty_shock</t>
   </si>
@@ -41,24 +41,6 @@
   </si>
   <si>
     <t>ED8</t>
-  </si>
-  <si>
-    <t>..</t>
-  </si>
-  <si>
-    <t>.</t>
-  </si>
-  <si>
-    <t>.....</t>
-  </si>
-  <si>
-    <t>...</t>
-  </si>
-  <si>
-    <t>....</t>
-  </si>
-  <si>
-    <t>......</t>
   </si>
 </sst>
 </file>
@@ -471,22 +453,16 @@
         <v>0.08219131506357374</v>
       </c>
       <c r="E2">
-        <v>0.6718374370814696</v>
+        <v>0.9565139767498894</v>
       </c>
       <c r="F2">
-        <v>0.5687995778620861</v>
+        <v>0.4775509216430419</v>
       </c>
       <c r="G2">
         <v>0</v>
-      </c>
-      <c r="H2" t="s">
-        <v>9</v>
       </c>
       <c r="I2">
         <v>-0.02</v>
-      </c>
-      <c r="J2" t="s">
-        <v>9</v>
       </c>
     </row>
     <row r="3" spans="1:10">
@@ -503,22 +479,16 @@
         <v>-0.8033668128521843</v>
       </c>
       <c r="E3">
-        <v>-0.443722178074067</v>
+        <v>0.3936084977691133</v>
       </c>
       <c r="F3">
-        <v>0.1733334372493402</v>
+        <v>0.7766929674223948</v>
       </c>
       <c r="G3">
         <v>0</v>
-      </c>
-      <c r="H3" t="s">
-        <v>10</v>
       </c>
       <c r="I3">
         <v>0.05</v>
-      </c>
-      <c r="J3" t="s">
-        <v>10</v>
       </c>
     </row>
     <row r="4" spans="1:10">
@@ -535,22 +505,16 @@
         <v>-0.06342931643641031</v>
       </c>
       <c r="E4">
-        <v>-0.3059591288434376</v>
+        <v>-0.2925735740499958</v>
       </c>
       <c r="F4">
-        <v>0.1569087587144425</v>
+        <v>0.4232579754683476</v>
       </c>
       <c r="G4">
         <v>0</v>
-      </c>
-      <c r="H4" t="s">
-        <v>9</v>
       </c>
       <c r="I4">
         <v>0.02</v>
-      </c>
-      <c r="J4" t="s">
-        <v>9</v>
       </c>
     </row>
     <row r="5" spans="1:10">
@@ -567,22 +531,16 @@
         <v>-0.7353396084563272</v>
       </c>
       <c r="E5">
-        <v>-0.2530470043137026</v>
+        <v>0.4673983445147144</v>
       </c>
       <c r="F5">
-        <v>-0.2022026909218307</v>
+        <v>0.08121974753313624</v>
       </c>
       <c r="G5">
         <v>0</v>
-      </c>
-      <c r="H5" t="s">
-        <v>11</v>
       </c>
       <c r="I5">
         <v>-0.54</v>
-      </c>
-      <c r="J5" t="s">
-        <v>11</v>
       </c>
     </row>
     <row r="6" spans="1:10">
@@ -599,22 +557,16 @@
         <v>0.4467189171490796</v>
       </c>
       <c r="E6">
-        <v>0.7309460509669714</v>
+        <v>0.56050629428272</v>
       </c>
       <c r="F6">
-        <v>0.3898820282244412</v>
+        <v>0.04863406108487361</v>
       </c>
       <c r="G6">
         <v>0</v>
-      </c>
-      <c r="H6" t="s">
-        <v>12</v>
       </c>
       <c r="I6">
         <v>-0.09</v>
-      </c>
-      <c r="J6" t="s">
-        <v>12</v>
       </c>
     </row>
     <row r="7" spans="1:10">
@@ -631,22 +583,16 @@
         <v>-0.7128309629173797</v>
       </c>
       <c r="E7">
-        <v>-0.4290576710591505</v>
+        <v>0.129194279352409</v>
       </c>
       <c r="F7">
-        <v>-0.4844485134375907</v>
+        <v>-0.261434301476444</v>
       </c>
       <c r="G7">
         <v>0</v>
-      </c>
-      <c r="H7" t="s">
-        <v>12</v>
       </c>
       <c r="I7">
         <v>-0.37</v>
-      </c>
-      <c r="J7" t="s">
-        <v>12</v>
       </c>
     </row>
     <row r="8" spans="1:10">
@@ -663,22 +609,16 @@
         <v>-0.1831355617516715</v>
       </c>
       <c r="E8">
-        <v>-0.1568865381526172</v>
+        <v>0.1942500818286506</v>
       </c>
       <c r="F8">
-        <v>0.7010402339080144</v>
+        <v>1.211551429059542</v>
       </c>
       <c r="G8">
         <v>0</v>
-      </c>
-      <c r="H8" t="s">
-        <v>13</v>
       </c>
       <c r="I8">
         <v>0.11</v>
-      </c>
-      <c r="J8" t="s">
-        <v>13</v>
       </c>
     </row>
     <row r="9" spans="1:10">
@@ -695,22 +635,16 @@
         <v>0.5708320911858327</v>
       </c>
       <c r="E9">
-        <v>0.54916502627464</v>
+        <v>0.1500066550611886</v>
       </c>
       <c r="F9">
-        <v>0.3083741852989822</v>
+        <v>-0.0210685812275678</v>
       </c>
       <c r="G9">
         <v>1.077778267687214</v>
       </c>
-      <c r="H9" t="s">
-        <v>12</v>
-      </c>
       <c r="I9">
         <v>0.05</v>
-      </c>
-      <c r="J9" t="s">
-        <v>12</v>
       </c>
     </row>
     <row r="10" spans="1:10">
@@ -727,22 +661,16 @@
         <v>-1.715001291582267</v>
       </c>
       <c r="E10">
-        <v>-1.846626584761373</v>
+        <v>-0.6902596369625047</v>
       </c>
       <c r="F10">
-        <v>-0.8393814818428597</v>
+        <v>0.3004308555947794</v>
       </c>
       <c r="G10">
         <v>0</v>
-      </c>
-      <c r="H10" t="s">
-        <v>9</v>
       </c>
       <c r="I10">
         <v>0.05</v>
-      </c>
-      <c r="J10" t="s">
-        <v>9</v>
       </c>
     </row>
     <row r="11" spans="1:10">
@@ -759,22 +687,16 @@
         <v>-0.2198184967270348</v>
       </c>
       <c r="E11">
-        <v>-0.4248102234214148</v>
+        <v>-0.3740961954527939</v>
       </c>
       <c r="F11">
-        <v>-0.2330706450662388</v>
+        <v>-0.05182807146337168</v>
       </c>
       <c r="G11">
         <v>0</v>
-      </c>
-      <c r="H11" t="s">
-        <v>13</v>
       </c>
       <c r="I11">
         <v>0.04000000000000001</v>
-      </c>
-      <c r="J11" t="s">
-        <v>13</v>
       </c>
     </row>
     <row r="12" spans="1:10">
@@ -791,22 +713,16 @@
         <v>-0.1705846726117453</v>
       </c>
       <c r="E12">
-        <v>0.2429131945234848</v>
+        <v>0.5154106935036182</v>
       </c>
       <c r="F12">
-        <v>-0.03395571191930713</v>
+        <v>-0.1222365140657953</v>
       </c>
       <c r="G12">
         <v>0</v>
-      </c>
-      <c r="H12" t="s">
-        <v>13</v>
       </c>
       <c r="I12">
         <v>-0.06</v>
-      </c>
-      <c r="J12" t="s">
-        <v>13</v>
       </c>
     </row>
     <row r="13" spans="1:10">
@@ -823,22 +739,16 @@
         <v>0.3960883912871317</v>
       </c>
       <c r="E13">
-        <v>0.4205997336707973</v>
+        <v>0.004561877327710073</v>
       </c>
       <c r="F13">
-        <v>-0.3490853025182278</v>
+        <v>-0.8909249387018572</v>
       </c>
       <c r="G13">
         <v>0</v>
       </c>
-      <c r="H13" t="s">
-        <v>9</v>
-      </c>
       <c r="I13">
         <v>0</v>
-      </c>
-      <c r="J13" t="s">
-        <v>9</v>
       </c>
     </row>
     <row r="14" spans="1:10">
@@ -855,22 +765,16 @@
         <v>0.6942281038026742</v>
       </c>
       <c r="E14">
-        <v>0.9982504137651925</v>
+        <v>0.4902022652606293</v>
       </c>
       <c r="F14">
-        <v>-0.1206190505781597</v>
+        <v>-0.9545470269071238</v>
       </c>
       <c r="G14">
         <v>0</v>
-      </c>
-      <c r="H14" t="s">
-        <v>9</v>
       </c>
       <c r="I14">
         <v>-0.03</v>
-      </c>
-      <c r="J14" t="s">
-        <v>9</v>
       </c>
     </row>
     <row r="15" spans="1:10">
@@ -887,22 +791,16 @@
         <v>0.4813416094932091</v>
       </c>
       <c r="E15">
-        <v>0.1803878376861855</v>
+        <v>-0.2215139431965063</v>
       </c>
       <c r="F15">
-        <v>0.3713963672334835</v>
+        <v>0.3020486735680512</v>
       </c>
       <c r="G15">
         <v>1.01705425996093</v>
       </c>
-      <c r="H15" t="s">
-        <v>12</v>
-      </c>
       <c r="I15">
         <v>-0.14</v>
-      </c>
-      <c r="J15" t="s">
-        <v>12</v>
       </c>
     </row>
     <row r="16" spans="1:10">
@@ -919,25 +817,19 @@
         <v>-0.02712013423335486</v>
       </c>
       <c r="E16">
-        <v>0.2957789287724284</v>
+        <v>0.5089129120344005</v>
       </c>
       <c r="F16">
-        <v>0.3010666535752355</v>
+        <v>0.3089985062411006</v>
       </c>
       <c r="G16">
         <v>1.628562764983808</v>
       </c>
-      <c r="H16" t="s">
-        <v>11</v>
-      </c>
       <c r="I16">
         <v>0.19</v>
       </c>
-      <c r="J16" t="s">
-        <v>11</v>
-      </c>
-    </row>
-    <row r="17" spans="1:10">
+    </row>
+    <row r="17" spans="1:9">
       <c r="A17" s="2">
         <v>32142</v>
       </c>
@@ -951,25 +843,19 @@
         <v>-0.5472471082872141</v>
       </c>
       <c r="E17">
-        <v>0.1599001655098287</v>
+        <v>1.014721135552556</v>
       </c>
       <c r="F17">
-        <v>0.5922217981853898</v>
+        <v>1.002945244089221</v>
       </c>
       <c r="G17">
         <v>0</v>
-      </c>
-      <c r="H17" t="s">
-        <v>13</v>
       </c>
       <c r="I17">
         <v>0.35</v>
       </c>
-      <c r="J17" t="s">
-        <v>13</v>
-      </c>
-    </row>
-    <row r="18" spans="1:10">
+    </row>
+    <row r="18" spans="1:9">
       <c r="A18" s="2">
         <v>32233</v>
       </c>
@@ -983,25 +869,19 @@
         <v>-0.2825210564843113</v>
       </c>
       <c r="E18">
-        <v>-0.8235882711962188</v>
+        <v>-0.9381781063155095</v>
       </c>
       <c r="F18">
-        <v>-0.6173021735919108</v>
+        <v>-0.4012877821129149</v>
       </c>
       <c r="G18">
         <v>0</v>
-      </c>
-      <c r="H18" t="s">
-        <v>12</v>
       </c>
       <c r="I18">
         <v>-0.01</v>
       </c>
-      <c r="J18" t="s">
-        <v>12</v>
-      </c>
-    </row>
-    <row r="19" spans="1:10">
+    </row>
+    <row r="19" spans="1:9">
       <c r="A19" s="2">
         <v>32324</v>
       </c>
@@ -1015,25 +895,19 @@
         <v>0.224660219419658</v>
       </c>
       <c r="E19">
-        <v>1.257696960566736</v>
+        <v>1.595734517977565</v>
       </c>
       <c r="F19">
-        <v>0.6509894621143992</v>
+        <v>0.2410366384349757</v>
       </c>
       <c r="G19">
         <v>0</v>
-      </c>
-      <c r="H19" t="s">
-        <v>13</v>
       </c>
       <c r="I19">
         <v>0.08</v>
       </c>
-      <c r="J19" t="s">
-        <v>13</v>
-      </c>
-    </row>
-    <row r="20" spans="1:10">
+    </row>
+    <row r="20" spans="1:9">
       <c r="A20" s="2">
         <v>32416</v>
       </c>
@@ -1047,25 +921,19 @@
         <v>0.490980495126371</v>
       </c>
       <c r="E20">
-        <v>-0.2517970989260997</v>
+        <v>-0.9767941295055254</v>
       </c>
       <c r="F20">
-        <v>-0.2412739974416137</v>
+        <v>-0.401518332691153</v>
       </c>
       <c r="G20">
         <v>0</v>
-      </c>
-      <c r="H20" t="s">
-        <v>11</v>
       </c>
       <c r="I20">
         <v>0.17</v>
       </c>
-      <c r="J20" t="s">
-        <v>11</v>
-      </c>
-    </row>
-    <row r="21" spans="1:10">
+    </row>
+    <row r="21" spans="1:9">
       <c r="A21" s="2">
         <v>32508</v>
       </c>
@@ -1079,10 +947,10 @@
         <v>-0.3201184599859809</v>
       </c>
       <c r="E21">
-        <v>0.6507731172280301</v>
+        <v>1.375666529456898</v>
       </c>
       <c r="F21">
-        <v>0.4818672163022656</v>
+        <v>0.4954169530545244</v>
       </c>
       <c r="G21">
         <v>0</v>
@@ -1093,11 +961,8 @@
       <c r="I21">
         <v>0.05</v>
       </c>
-      <c r="J21" t="s">
-        <v>13</v>
-      </c>
-    </row>
-    <row r="22" spans="1:10">
+    </row>
+    <row r="22" spans="1:9">
       <c r="A22" s="2">
         <v>32598</v>
       </c>
@@ -1111,10 +976,10 @@
         <v>-0.02701594773041348</v>
       </c>
       <c r="E22">
-        <v>0.1745808995512717</v>
+        <v>0.2746190525551792</v>
       </c>
       <c r="F22">
-        <v>0.03494120984737648</v>
+        <v>-0.03066039515548702</v>
       </c>
       <c r="G22">
         <v>1.993475330405829</v>
@@ -1125,11 +990,8 @@
       <c r="I22">
         <v>0.07000000000000001</v>
       </c>
-      <c r="J22" t="s">
-        <v>11</v>
-      </c>
-    </row>
-    <row r="23" spans="1:10">
+    </row>
+    <row r="23" spans="1:9">
       <c r="A23" s="2">
         <v>32689</v>
       </c>
@@ -1143,10 +1005,10 @@
         <v>0.7085043110072846</v>
       </c>
       <c r="E23">
-        <v>0.3213612358947009</v>
+        <v>-0.3503837241676325</v>
       </c>
       <c r="F23">
-        <v>0.1808555454125741</v>
+        <v>-0.1408023931169053</v>
       </c>
       <c r="G23">
         <v>2.010622206645562</v>
@@ -1157,11 +1019,8 @@
       <c r="I23">
         <v>-0.07000000000000001</v>
       </c>
-      <c r="J23" t="s">
-        <v>9</v>
-      </c>
-    </row>
-    <row r="24" spans="1:10">
+    </row>
+    <row r="24" spans="1:9">
       <c r="A24" s="2">
         <v>32781</v>
       </c>
@@ -1175,10 +1034,10 @@
         <v>-1.045312939833492</v>
       </c>
       <c r="E24">
-        <v>-0.8350283714911156</v>
+        <v>0.03777412845018321</v>
       </c>
       <c r="F24">
-        <v>-0.2535074025062436</v>
+        <v>0.4203192077762569</v>
       </c>
       <c r="G24">
         <v>0</v>
@@ -1189,11 +1048,8 @@
       <c r="I24">
         <v>-0.07000000000000001</v>
       </c>
-      <c r="J24" t="s">
-        <v>12</v>
-      </c>
-    </row>
-    <row r="25" spans="1:10">
+    </row>
+    <row r="25" spans="1:9">
       <c r="A25" s="2">
         <v>32873</v>
       </c>
@@ -1207,10 +1063,10 @@
         <v>0.343872973270769</v>
       </c>
       <c r="E25">
-        <v>0.1144845598460189</v>
+        <v>-0.2938546935760876</v>
       </c>
       <c r="F25">
-        <v>-0.1645066104394469</v>
+        <v>-0.4294215844772615</v>
       </c>
       <c r="G25">
         <v>0.05811786702709119</v>
@@ -1221,11 +1077,8 @@
       <c r="I25">
         <v>-0.07000000000000001</v>
       </c>
-      <c r="J25" t="s">
-        <v>11</v>
-      </c>
-    </row>
-    <row r="26" spans="1:10">
+    </row>
+    <row r="26" spans="1:9">
       <c r="A26" s="2">
         <v>32963</v>
       </c>
@@ -1239,10 +1092,10 @@
         <v>1.21490947885941</v>
       </c>
       <c r="E26">
-        <v>1.206519929485727</v>
+        <v>0.4868215156249125</v>
       </c>
       <c r="F26">
-        <v>1.088865801845139</v>
+        <v>0.5920507584650876</v>
       </c>
       <c r="G26">
         <v>1.812273244531602</v>
@@ -1253,11 +1106,8 @@
       <c r="I26">
         <v>-0.02</v>
       </c>
-      <c r="J26" t="s">
-        <v>9</v>
-      </c>
-    </row>
-    <row r="27" spans="1:10">
+    </row>
+    <row r="27" spans="1:9">
       <c r="A27" s="2">
         <v>33054</v>
       </c>
@@ -1271,10 +1121,10 @@
         <v>0.05900124525253303</v>
       </c>
       <c r="E27">
-        <v>-0.5737828253131996</v>
+        <v>-0.8621203952868864</v>
       </c>
       <c r="F27">
-        <v>-0.09421030269370378</v>
+        <v>0.1423709948940912</v>
       </c>
       <c r="G27">
         <v>0</v>
@@ -1285,11 +1135,8 @@
       <c r="I27">
         <v>-0.02</v>
       </c>
-      <c r="J27" t="s">
-        <v>10</v>
-      </c>
-    </row>
-    <row r="28" spans="1:10">
+    </row>
+    <row r="28" spans="1:9">
       <c r="A28" s="2">
         <v>33146</v>
       </c>
@@ -1303,10 +1150,10 @@
         <v>1.656339652947235</v>
       </c>
       <c r="E28">
-        <v>0.9435611099530433</v>
+        <v>-0.5136271376524492</v>
       </c>
       <c r="F28">
-        <v>0.6011393648836355</v>
+        <v>-0.1607740356762762</v>
       </c>
       <c r="G28">
         <v>5.479579345864195</v>
@@ -1317,11 +1164,8 @@
       <c r="I28">
         <v>-0.01</v>
       </c>
-      <c r="J28" t="s">
-        <v>12</v>
-      </c>
-    </row>
-    <row r="29" spans="1:10">
+    </row>
+    <row r="29" spans="1:9">
       <c r="A29" s="2">
         <v>33238</v>
       </c>
@@ -1335,10 +1179,10 @@
         <v>-0.6104298110569003</v>
       </c>
       <c r="E29">
-        <v>-0.9023160602393351</v>
+        <v>-0.9449752770357203</v>
       </c>
       <c r="F29">
-        <v>-1.671074795694973</v>
+        <v>-1.846866676431664</v>
       </c>
       <c r="G29">
         <v>1.638326754690848</v>
@@ -1349,11 +1193,8 @@
       <c r="I29">
         <v>3.469446951953614e-18</v>
       </c>
-      <c r="J29" t="s">
-        <v>11</v>
-      </c>
-    </row>
-    <row r="30" spans="1:10">
+    </row>
+    <row r="30" spans="1:9">
       <c r="A30" s="2">
         <v>33328</v>
       </c>
@@ -1367,10 +1208,10 @@
         <v>-0.9325006627717529</v>
       </c>
       <c r="E30">
-        <v>-1.292866140512166</v>
+        <v>-0.9805913032751121</v>
       </c>
       <c r="F30">
-        <v>-1.265183003998403</v>
+        <v>-0.9111886015538887</v>
       </c>
       <c r="G30">
         <v>0</v>
@@ -1381,11 +1222,8 @@
       <c r="I30">
         <v>-0.19</v>
       </c>
-      <c r="J30" t="s">
-        <v>11</v>
-      </c>
-    </row>
-    <row r="31" spans="1:10">
+    </row>
+    <row r="31" spans="1:9">
       <c r="A31" s="2">
         <v>33419</v>
       </c>
@@ -1399,10 +1237,10 @@
         <v>-0.01875591122276032</v>
       </c>
       <c r="E31">
-        <v>0.1053604648094053</v>
+        <v>0.3355959131328233</v>
       </c>
       <c r="F31">
-        <v>0.637956657064622</v>
+        <v>0.9193024317393198</v>
       </c>
       <c r="G31">
         <v>0</v>
@@ -1413,11 +1251,8 @@
       <c r="I31">
         <v>-0.13</v>
       </c>
-      <c r="J31" t="s">
-        <v>9</v>
-      </c>
-    </row>
-    <row r="32" spans="1:10">
+    </row>
+    <row r="32" spans="1:9">
       <c r="A32" s="2">
         <v>33511</v>
       </c>
@@ -1431,10 +1266,10 @@
         <v>-0.1364564529769891</v>
       </c>
       <c r="E32">
-        <v>-0.07618127330398852</v>
+        <v>0.04258255957274473</v>
       </c>
       <c r="F32">
-        <v>-0.05621161823182266</v>
+        <v>0.002260278499669009</v>
       </c>
       <c r="G32">
         <v>0</v>
@@ -1444,9 +1279,6 @@
       </c>
       <c r="I32">
         <v>-0.02</v>
-      </c>
-      <c r="J32" t="s">
-        <v>13</v>
       </c>
     </row>
     <row r="33" spans="1:10">
@@ -1463,10 +1295,10 @@
         <v>0.5169639073146303</v>
       </c>
       <c r="E33">
-        <v>-0.03183209996397868</v>
+        <v>-0.7211919976237502</v>
       </c>
       <c r="F33">
-        <v>-0.2717078026159263</v>
+        <v>-0.573934170274267</v>
       </c>
       <c r="G33">
         <v>0</v>
@@ -1476,9 +1308,6 @@
       </c>
       <c r="I33">
         <v>-0.17</v>
-      </c>
-      <c r="J33" t="s">
-        <v>14</v>
       </c>
     </row>
     <row r="34" spans="1:10">
@@ -1495,10 +1324,10 @@
         <v>0.1870021693723587</v>
       </c>
       <c r="E34">
-        <v>-0.3923866043427153</v>
+        <v>-0.5754437355095563</v>
       </c>
       <c r="F34">
-        <v>0.6218026188210884</v>
+        <v>1.089119805625075</v>
       </c>
       <c r="G34">
         <v>0</v>
@@ -1508,9 +1337,6 @@
       </c>
       <c r="I34">
         <v>0.01</v>
-      </c>
-      <c r="J34" t="s">
-        <v>10</v>
       </c>
     </row>
     <row r="35" spans="1:10">
@@ -1527,10 +1353,10 @@
         <v>-0.1129622988416226</v>
       </c>
       <c r="E35">
-        <v>0.3819794437132398</v>
+        <v>0.774350726360864</v>
       </c>
       <c r="F35">
-        <v>0.484494546820854</v>
+        <v>0.5712556198961964</v>
       </c>
       <c r="G35">
         <v>0</v>
@@ -1540,9 +1366,6 @@
       </c>
       <c r="I35">
         <v>-0.14</v>
-      </c>
-      <c r="J35" t="s">
-        <v>12</v>
       </c>
     </row>
     <row r="36" spans="1:10">
@@ -1559,10 +1382,10 @@
         <v>0.1118806781486146</v>
       </c>
       <c r="E36">
-        <v>-0.2689380568231304</v>
+        <v>-0.5326340483166994</v>
       </c>
       <c r="F36">
-        <v>-0.1548688003318482</v>
+        <v>-0.1304621910520799</v>
       </c>
       <c r="G36">
         <v>0</v>
@@ -1572,9 +1395,6 @@
       </c>
       <c r="I36">
         <v>0.04999999999999999</v>
-      </c>
-      <c r="J36" t="s">
-        <v>12</v>
       </c>
     </row>
     <row r="37" spans="1:10">
@@ -1591,10 +1411,10 @@
         <v>-0.01666035472855869</v>
       </c>
       <c r="E37">
-        <v>0.2038277623656937</v>
+        <v>0.2945531658420256</v>
       </c>
       <c r="F37">
-        <v>0.008825274185548904</v>
+        <v>-0.08948499879474955</v>
       </c>
       <c r="G37">
         <v>0</v>
@@ -1604,9 +1424,6 @@
       </c>
       <c r="I37">
         <v>0</v>
-      </c>
-      <c r="J37" t="s">
-        <v>12</v>
       </c>
     </row>
     <row r="38" spans="1:10">
@@ -1623,10 +1440,10 @@
         <v>-0.6265055935167666</v>
       </c>
       <c r="E38">
-        <v>-0.3748507466358204</v>
+        <v>-0.1170493257046984</v>
       </c>
       <c r="F38">
-        <v>-1.288712442503894</v>
+        <v>-1.541675825576774</v>
       </c>
       <c r="G38">
         <v>0</v>
@@ -1636,9 +1453,6 @@
       </c>
       <c r="I38">
         <v>0.04</v>
-      </c>
-      <c r="J38" t="s">
-        <v>9</v>
       </c>
     </row>
     <row r="39" spans="1:10">
@@ -1655,10 +1469,10 @@
         <v>-0.5775443421097876</v>
       </c>
       <c r="E39">
-        <v>-0.02497612625307527</v>
+        <v>0.3982968401852631</v>
       </c>
       <c r="F39">
-        <v>-0.9022624370971843</v>
+        <v>-1.15804596368975</v>
       </c>
       <c r="G39">
         <v>0</v>
@@ -1668,9 +1482,6 @@
       </c>
       <c r="I39">
         <v>-0.01</v>
-      </c>
-      <c r="J39" t="s">
-        <v>10</v>
       </c>
     </row>
     <row r="40" spans="1:10">
@@ -1687,10 +1498,10 @@
         <v>-0.7046005136171138</v>
       </c>
       <c r="E40">
-        <v>-0.6708279712567935</v>
+        <v>-0.2902568799458474</v>
       </c>
       <c r="F40">
-        <v>-0.8035982798349249</v>
+        <v>-0.6201723087773076</v>
       </c>
       <c r="G40">
         <v>0</v>
@@ -1700,9 +1511,6 @@
       </c>
       <c r="I40">
         <v>-0.04</v>
-      </c>
-      <c r="J40" t="s">
-        <v>12</v>
       </c>
     </row>
     <row r="41" spans="1:10">
@@ -1719,10 +1527,10 @@
         <v>0.2868856200598068</v>
       </c>
       <c r="E41">
-        <v>0.8776327897530131</v>
+        <v>1.086710355961984</v>
       </c>
       <c r="F41">
-        <v>0.9177866282181264</v>
+        <v>0.8273843939759105</v>
       </c>
       <c r="G41">
         <v>0</v>
@@ -1732,9 +1540,6 @@
       </c>
       <c r="I41">
         <v>-0.08</v>
-      </c>
-      <c r="J41" t="s">
-        <v>9</v>
       </c>
     </row>
     <row r="42" spans="1:10">
@@ -1751,10 +1556,10 @@
         <v>-0.3879038903920575</v>
       </c>
       <c r="E42">
-        <v>-0.361604124843841</v>
+        <v>-0.04857485617621306</v>
       </c>
       <c r="F42">
-        <v>-0.06964201318996956</v>
+        <v>0.220657593417373</v>
       </c>
       <c r="G42">
         <v>0</v>
@@ -1783,10 +1588,10 @@
         <v>-0.6562541713035794</v>
       </c>
       <c r="E43">
-        <v>0.4882140152430888</v>
+        <v>1.417868992199089</v>
       </c>
       <c r="F43">
-        <v>-0.01221443398649025</v>
+        <v>-0.05253420342147352</v>
       </c>
       <c r="G43">
         <v>0</v>
@@ -1815,10 +1620,10 @@
         <v>-0.08392035323546346</v>
       </c>
       <c r="E44">
-        <v>-0.1584176787670138</v>
+        <v>-0.352768080378951</v>
       </c>
       <c r="F44">
-        <v>-0.8831230517689479</v>
+        <v>-1.228013644172807</v>
       </c>
       <c r="G44">
         <v>0.7641246571096181</v>
@@ -1847,10 +1652,10 @@
         <v>-0.253493300328674</v>
       </c>
       <c r="E45">
-        <v>-0.3753552217224306</v>
+        <v>-0.1697054387516238</v>
       </c>
       <c r="F45">
-        <v>0.1319724686040775</v>
+        <v>0.4878851298075308</v>
       </c>
       <c r="G45">
         <v>0</v>
@@ -1879,10 +1684,10 @@
         <v>-0.1674783156835627</v>
       </c>
       <c r="E46">
-        <v>0.01058957077138087</v>
+        <v>0.1761015964440342</v>
       </c>
       <c r="F46">
-        <v>-0.125895996707908</v>
+        <v>-0.1391351718412736</v>
       </c>
       <c r="G46">
         <v>0</v>
@@ -1911,10 +1716,10 @@
         <v>0.2274668707012617</v>
       </c>
       <c r="E47">
-        <v>-0.2566372245964842</v>
+        <v>-0.6911249876276356</v>
       </c>
       <c r="F47">
-        <v>-0.3013863617821947</v>
+        <v>-0.3994070222179424</v>
       </c>
       <c r="G47">
         <v>0.2839548654467709</v>
@@ -1943,10 +1748,10 @@
         <v>-0.9581625532112585</v>
       </c>
       <c r="E48">
-        <v>0.2707759169149322</v>
+        <v>1.409186458591259</v>
       </c>
       <c r="F48">
-        <v>-0.2750979893990391</v>
+        <v>-0.2318693903265908</v>
       </c>
       <c r="G48">
         <v>0</v>
@@ -1975,10 +1780,10 @@
         <v>-0.1054893579250303</v>
       </c>
       <c r="E49">
-        <v>-0.5397982260964493</v>
+        <v>-0.737215283385475</v>
       </c>
       <c r="F49">
-        <v>-0.5119159902270836</v>
+        <v>-0.4534915605263012</v>
       </c>
       <c r="G49">
         <v>0</v>
@@ -2007,10 +1812,10 @@
         <v>0.6434061687713341</v>
       </c>
       <c r="E50">
-        <v>0.4402587560022781</v>
+        <v>-0.05117457405285568</v>
       </c>
       <c r="F50">
-        <v>0.4171470816465249</v>
+        <v>0.1771721334967276</v>
       </c>
       <c r="G50">
         <v>1.844170999062691</v>
@@ -2039,10 +1844,10 @@
         <v>-0.01613125450140507</v>
       </c>
       <c r="E51">
-        <v>0.680013205461122</v>
+        <v>1.212896519179752</v>
       </c>
       <c r="F51">
-        <v>1.050380940960863</v>
+        <v>1.238558833623084</v>
       </c>
       <c r="G51">
         <v>2.510993297856251</v>
@@ -2071,10 +1876,10 @@
         <v>-0.3780018263286115</v>
       </c>
       <c r="E52">
-        <v>-0.267449114202252</v>
+        <v>-0.04956933182491211</v>
       </c>
       <c r="F52">
-        <v>-0.4957748388924228</v>
+        <v>-0.4801886878951207</v>
       </c>
       <c r="G52">
         <v>0.4504616443464192</v>
@@ -2103,10 +1908,10 @@
         <v>-0.2308944974844325</v>
       </c>
       <c r="E53">
-        <v>0.1811112114459105</v>
+        <v>0.431680160787953</v>
       </c>
       <c r="F53">
-        <v>-0.2986062095340935</v>
+        <v>-0.4704856263688061</v>
       </c>
       <c r="G53">
         <v>0.9495341746291633</v>
@@ -2135,10 +1940,10 @@
         <v>-0.978441048286343</v>
       </c>
       <c r="E54">
-        <v>-0.7609292213701201</v>
+        <v>-0.1214869624225576</v>
       </c>
       <c r="F54">
-        <v>-0.9188628299417924</v>
+        <v>-0.6528306289954676</v>
       </c>
       <c r="G54">
         <v>0</v>
@@ -2167,10 +1972,10 @@
         <v>-0.4714796793388653</v>
       </c>
       <c r="E55">
-        <v>-0.2237560785015816</v>
+        <v>0.4195818196131459</v>
       </c>
       <c r="F55">
-        <v>0.6172087797718</v>
+        <v>1.219254642289617</v>
       </c>
       <c r="G55">
         <v>0</v>
@@ -2199,10 +2004,10 @@
         <v>-0.03418044688733057</v>
       </c>
       <c r="E56">
-        <v>0.1583038929224518</v>
+        <v>0.3947666037038822</v>
       </c>
       <c r="F56">
-        <v>0.5282236689927975</v>
+        <v>0.7297294673994226</v>
       </c>
       <c r="G56">
         <v>0</v>
@@ -2231,10 +2036,10 @@
         <v>-0.2821954530122913</v>
       </c>
       <c r="E57">
-        <v>-0.3475411134687255</v>
+        <v>-0.2139037484156456</v>
       </c>
       <c r="F57">
-        <v>-0.2928328832333247</v>
+        <v>-0.1622802789971164</v>
       </c>
       <c r="G57">
         <v>0</v>
@@ -2263,10 +2068,10 @@
         <v>-0.7691412498660385</v>
       </c>
       <c r="E58">
-        <v>-0.4570957386783783</v>
+        <v>0.1799978292385116</v>
       </c>
       <c r="F58">
-        <v>-0.4016845522323254</v>
+        <v>-0.1013703267930604</v>
       </c>
       <c r="G58">
         <v>0</v>
@@ -2295,10 +2100,10 @@
         <v>-0.05849622409384361</v>
       </c>
       <c r="E59">
-        <v>-0.03763653762919174</v>
+        <v>-0.01938592525571125</v>
       </c>
       <c r="F59">
-        <v>-0.1385352342572867</v>
+        <v>-0.1701975086876201</v>
       </c>
       <c r="G59">
         <v>0</v>
@@ -2327,10 +2132,10 @@
         <v>0.170822166233998</v>
       </c>
       <c r="E60">
-        <v>-0.1001764502888186</v>
+        <v>-0.2009403509715288</v>
       </c>
       <c r="F60">
-        <v>0.4912955840594944</v>
+        <v>0.7407332689609439</v>
       </c>
       <c r="G60">
         <v>0</v>
@@ -2359,10 +2164,10 @@
         <v>-0.1069524395505569</v>
       </c>
       <c r="E61">
-        <v>0.7974371869546627</v>
+        <v>1.395283686144378</v>
       </c>
       <c r="F61">
-        <v>0.7512016668031165</v>
+        <v>0.7528608487016704</v>
       </c>
       <c r="G61">
         <v>0</v>
@@ -2391,10 +2196,10 @@
         <v>-0.1649875441025868</v>
       </c>
       <c r="E62">
-        <v>-1.109263611625303</v>
+        <v>-1.408915858719181</v>
       </c>
       <c r="F62">
-        <v>-0.4363786692740977</v>
+        <v>-0.01474436849369443</v>
       </c>
       <c r="G62">
         <v>0</v>
@@ -2423,10 +2228,10 @@
         <v>0.1355589162355165</v>
       </c>
       <c r="E63">
-        <v>0.4544609488318122</v>
+        <v>0.4822678809072474</v>
       </c>
       <c r="F63">
-        <v>0.1218433153603056</v>
+        <v>-0.10387225860512</v>
       </c>
       <c r="G63">
         <v>2.959857470662012</v>
@@ -2455,10 +2260,10 @@
         <v>0.7590274977140816</v>
       </c>
       <c r="E64">
-        <v>0.7199157247700718</v>
+        <v>0.2768158699382891</v>
       </c>
       <c r="F64">
-        <v>0.7466911847860979</v>
+        <v>0.4888127328169368</v>
       </c>
       <c r="G64">
         <v>2.96392508179641</v>
@@ -2487,10 +2292,10 @@
         <v>-0.03036556531488183</v>
       </c>
       <c r="E65">
-        <v>0.0336545564195351</v>
+        <v>0.2779644255493164</v>
       </c>
       <c r="F65">
-        <v>0.7292097139223345</v>
+        <v>1.100124995900282</v>
       </c>
       <c r="G65">
         <v>1.138342902860217</v>
@@ -2519,10 +2324,10 @@
         <v>0.64738250964999</v>
       </c>
       <c r="E66">
-        <v>0.4395977890164288</v>
+        <v>-0.214492845055467</v>
       </c>
       <c r="F66">
-        <v>-0.1656920629910948</v>
+        <v>-0.7091187776767086</v>
       </c>
       <c r="G66">
         <v>1.958994806713817</v>
@@ -2551,10 +2356,10 @@
         <v>-0.1422465779359978</v>
       </c>
       <c r="E67">
-        <v>-0.2242669515919335</v>
+        <v>0.08626687337194944</v>
       </c>
       <c r="F67">
-        <v>0.8118954142936081</v>
+        <v>1.40174538129296</v>
       </c>
       <c r="G67">
         <v>1.603828708671828</v>
@@ -2583,10 +2388,10 @@
         <v>-0.2217968692235719</v>
       </c>
       <c r="E68">
-        <v>-0.4051339823545107</v>
+        <v>-0.4375469818868615</v>
       </c>
       <c r="F68">
-        <v>-0.5732418095541612</v>
+        <v>-0.5783176975610864</v>
       </c>
       <c r="G68">
         <v>1.591851077430585</v>
@@ -2615,10 +2420,10 @@
         <v>-0.1608719586148882</v>
       </c>
       <c r="E69">
-        <v>-0.6112384047181287</v>
+        <v>-0.6976491194003688</v>
       </c>
       <c r="F69">
-        <v>-0.2521789537937187</v>
+        <v>-0.001811810679628933</v>
       </c>
       <c r="G69">
         <v>0.3884698438449789</v>
@@ -2647,10 +2452,10 @@
         <v>-0.1069844364521345</v>
       </c>
       <c r="E70">
-        <v>-0.1677531233011494</v>
+        <v>-0.3234777253353051</v>
       </c>
       <c r="F70">
-        <v>-0.8285098106218147</v>
+        <v>-1.132135865709504</v>
       </c>
       <c r="G70">
         <v>0</v>
@@ -2679,10 +2484,10 @@
         <v>0.9924024046955395</v>
       </c>
       <c r="E71">
-        <v>-0.1042337582209656</v>
+        <v>-1.153747756135976</v>
       </c>
       <c r="F71">
-        <v>0.5437477629548739</v>
+        <v>0.5393569511519571</v>
       </c>
       <c r="G71">
         <v>0</v>
@@ -2711,10 +2516,10 @@
         <v>-0.7126789813412027</v>
       </c>
       <c r="E72">
-        <v>-1.136774766031891</v>
+        <v>-0.9146256725722562</v>
       </c>
       <c r="F72">
-        <v>-0.842447409932171</v>
+        <v>-0.4280628944137352</v>
       </c>
       <c r="G72">
         <v>0</v>
@@ -2743,10 +2548,10 @@
         <v>-1.002907376533911</v>
       </c>
       <c r="E73">
-        <v>-1.349547280636372</v>
+        <v>-0.7983399299623877</v>
       </c>
       <c r="F73">
-        <v>-0.6162559764495654</v>
+        <v>0.1289435274088505</v>
       </c>
       <c r="G73">
         <v>0</v>
@@ -2775,10 +2580,10 @@
         <v>0.8936351528551678</v>
       </c>
       <c r="E74">
-        <v>0.3630756989634116</v>
+        <v>-0.3378151742202298</v>
       </c>
       <c r="F74">
-        <v>0.8215558219702574</v>
+        <v>0.7463061807227001</v>
       </c>
       <c r="G74">
         <v>0</v>
@@ -2807,10 +2612,10 @@
         <v>0.3346717067417043</v>
       </c>
       <c r="E75">
-        <v>0.5103871895390811</v>
+        <v>0.2671573080826987</v>
       </c>
       <c r="F75">
-        <v>-0.08827959134981644</v>
+        <v>-0.5214703590788172</v>
       </c>
       <c r="G75">
         <v>0</v>
@@ -2839,10 +2644,10 @@
         <v>0.8349961405656444</v>
       </c>
       <c r="E76">
-        <v>-0.1976482905716547</v>
+        <v>-1.32741302996219</v>
       </c>
       <c r="F76">
-        <v>-0.3166991603664993</v>
+        <v>-0.6635268405890378</v>
       </c>
       <c r="G76">
         <v>1.133699809713123</v>
@@ -2871,10 +2676,10 @@
         <v>-0.4087347603955785</v>
       </c>
       <c r="E77">
-        <v>-0.3925265161935659</v>
+        <v>-0.2815308095079139</v>
       </c>
       <c r="F77">
-        <v>-0.8674374484660335</v>
+        <v>-0.9674501761068235</v>
       </c>
       <c r="G77">
         <v>0</v>
@@ -2903,10 +2708,10 @@
         <v>1.25526036176332</v>
       </c>
       <c r="E78">
-        <v>0.3798721525055418</v>
+        <v>-0.8009141167095559</v>
       </c>
       <c r="F78">
-        <v>0.5913421898080958</v>
+        <v>0.2630271787241</v>
       </c>
       <c r="G78">
         <v>2.666480949903399</v>
@@ -2935,10 +2740,10 @@
         <v>-1.878817377856121</v>
       </c>
       <c r="E79">
-        <v>-1.477365510655323</v>
+        <v>0.06456547078164618</v>
       </c>
       <c r="F79">
-        <v>-0.5840304655450976</v>
+        <v>0.5479494164180853</v>
       </c>
       <c r="G79">
         <v>0</v>
@@ -2967,10 +2772,10 @@
         <v>1.554278733993455</v>
       </c>
       <c r="E80">
-        <v>1.411995389381612</v>
+        <v>0.5645992732676416</v>
       </c>
       <c r="F80">
-        <v>1.82806114452915</v>
+        <v>1.488316830682545</v>
       </c>
       <c r="G80">
         <v>0</v>
@@ -2999,10 +2804,10 @@
         <v>-1.044110628208361</v>
       </c>
       <c r="E81">
-        <v>-0.8873342213900419</v>
+        <v>-0.1428635300002524</v>
       </c>
       <c r="F81">
-        <v>-0.6571126146486671</v>
+        <v>-0.1652528014868562</v>
       </c>
       <c r="G81">
         <v>0</v>
@@ -3031,10 +2836,10 @@
         <v>0.828707264877302</v>
       </c>
       <c r="E82">
-        <v>0.4133486022601277</v>
+        <v>-0.45355127760262</v>
       </c>
       <c r="F82">
-        <v>-0.135111228417548</v>
+        <v>-0.7111845253776778</v>
       </c>
       <c r="G82">
         <v>1.44145137487118</v>
@@ -3063,10 +2868,10 @@
         <v>0.2450785686373946</v>
       </c>
       <c r="E83">
-        <v>-0.1656347920801692</v>
+        <v>-0.5499186496889547</v>
       </c>
       <c r="F83">
-        <v>-0.1533192185591775</v>
+        <v>-0.2290802191411092</v>
       </c>
       <c r="G83">
         <v>2.332211655149826</v>
@@ -3095,10 +2900,10 @@
         <v>-0.5347418675693673</v>
       </c>
       <c r="E84">
-        <v>0.02629671837731579</v>
+        <v>0.6815120828247276</v>
       </c>
       <c r="F84">
-        <v>0.0756213963340075</v>
+        <v>0.2851775839815154</v>
       </c>
       <c r="G84">
         <v>2.533722552038431</v>
@@ -3127,10 +2932,10 @@
         <v>0.4349034910757798</v>
       </c>
       <c r="E85">
-        <v>0.4011298616692468</v>
+        <v>0.09196770900057716</v>
       </c>
       <c r="F85">
-        <v>0.237817989711316</v>
+        <v>-0.002482712473254496</v>
       </c>
       <c r="G85">
         <v>3.702878707826549</v>
@@ -3159,10 +2964,10 @@
         <v>-0.1050838202641348</v>
       </c>
       <c r="E86">
-        <v>-0.3023886260151615</v>
+        <v>-0.2412160383198744</v>
       </c>
       <c r="F86">
-        <v>0.148887922028014</v>
+        <v>0.42353099258011</v>
       </c>
       <c r="G86">
         <v>0.5602379884717499</v>
@@ -3191,10 +2996,10 @@
         <v>-0.9685911043285343</v>
       </c>
       <c r="E87">
-        <v>-0.536854603925174</v>
+        <v>0.2068745518304158</v>
       </c>
       <c r="F87">
-        <v>-0.7705840583635638</v>
+        <v>-0.5504293950442447</v>
       </c>
       <c r="G87">
         <v>0.8996662250563859</v>
@@ -3223,10 +3028,10 @@
         <v>3.312965098383626</v>
       </c>
       <c r="E88">
-        <v>2.365367665330806</v>
+        <v>-0.2541171347272043</v>
       </c>
       <c r="F88">
-        <v>1.696211857769768</v>
+        <v>0.1736996235644274</v>
       </c>
       <c r="G88">
         <v>2.588301040572271</v>
@@ -3255,10 +3060,10 @@
         <v>-3.049651387259017</v>
       </c>
       <c r="E89">
-        <v>-2.077567239728152</v>
+        <v>0.3377703388031585</v>
       </c>
       <c r="F89">
-        <v>-1.670947501402284</v>
+        <v>-0.3794799732754699</v>
       </c>
       <c r="G89">
         <v>0</v>
@@ -3287,10 +3092,10 @@
         <v>0.3153913038736469</v>
       </c>
       <c r="E90">
-        <v>0.854056574633284</v>
+        <v>0.9537242074185639</v>
       </c>
       <c r="F90">
-        <v>0.6662823402168874</v>
+        <v>0.4481143621275307</v>
       </c>
       <c r="G90">
         <v>0</v>
@@ -3319,10 +3124,10 @@
         <v>-0.4220851925867697</v>
       </c>
       <c r="E91">
-        <v>-0.9147347136656105</v>
+        <v>-1.079340140787219</v>
       </c>
       <c r="F91">
-        <v>-1.291750426710391</v>
+        <v>-1.329017990414922</v>
       </c>
       <c r="G91">
         <v>1.55417988427537</v>
@@ -3351,10 +3156,10 @@
         <v>-0.3572126674274089</v>
       </c>
       <c r="E92">
-        <v>-0.06611046976331159</v>
+        <v>0.191937746829564</v>
       </c>
       <c r="F92">
-        <v>-0.5086900353277756</v>
+        <v>-0.6142778870795653</v>
       </c>
       <c r="G92">
         <v>1.210779179881358</v>
@@ -3383,10 +3188,10 @@
         <v>-0.990000449888053</v>
       </c>
       <c r="E93">
-        <v>-0.705355683888293</v>
+        <v>0.1002405818196699</v>
       </c>
       <c r="F93">
-        <v>-0.4243976365171677</v>
+        <v>0.07257696282285821</v>
       </c>
       <c r="G93">
         <v>0</v>
@@ -3415,10 +3220,10 @@
         <v>0.7411595667700812</v>
       </c>
       <c r="E94">
-        <v>0.3447697883580222</v>
+        <v>-0.4241179307555147</v>
       </c>
       <c r="F94">
-        <v>-0.06600879415117689</v>
+        <v>-0.539496379241525</v>
       </c>
       <c r="G94">
         <v>0</v>
@@ -3447,10 +3252,10 @@
         <v>0.3695653748939855</v>
       </c>
       <c r="E95">
-        <v>0.4532457247171878</v>
+        <v>0.221068539562484</v>
       </c>
       <c r="F95">
-        <v>0.1746967040317416</v>
+        <v>-0.1036104657391762</v>
       </c>
       <c r="G95">
         <v>0</v>
@@ -3479,10 +3284,10 @@
         <v>0.1742664261348304</v>
       </c>
       <c r="E96">
-        <v>-0.4094151061216145</v>
+        <v>-0.7444649892321131</v>
       </c>
       <c r="F96">
-        <v>0.0265234377653899</v>
+        <v>0.1984179046065224</v>
       </c>
       <c r="G96">
         <v>1.904047410826543</v>
@@ -3511,10 +3316,10 @@
         <v>1.104115281538792</v>
       </c>
       <c r="E97">
-        <v>0.7480172512855695</v>
+        <v>-0.09072013521733732</v>
       </c>
       <c r="F97">
-        <v>0.7421232576010868</v>
+        <v>0.3479417151958263</v>
       </c>
       <c r="G97">
         <v>2.376943767352481</v>
@@ -3543,10 +3348,10 @@
         <v>-0.189241231193245</v>
       </c>
       <c r="E98">
-        <v>-0.638419463259427</v>
+        <v>-0.9656984589120812</v>
       </c>
       <c r="F98">
-        <v>-1.230689092380535</v>
+        <v>-1.463801977209248</v>
       </c>
       <c r="G98">
         <v>2.594403687794504</v>
@@ -3575,10 +3380,10 @@
         <v>2.00478375163709</v>
       </c>
       <c r="E99">
-        <v>1.294297006380971</v>
+        <v>-0.313627691759002</v>
       </c>
       <c r="F99">
-        <v>1.113246007367973</v>
+        <v>0.310021075163141</v>
       </c>
       <c r="G99">
         <v>2.750703966502953</v>
@@ -3607,10 +3412,10 @@
         <v>-0.9217369783175271</v>
       </c>
       <c r="E100">
-        <v>-1.569862815245259</v>
+        <v>-1.365305605245221</v>
       </c>
       <c r="F100">
-        <v>-1.270990241968123</v>
+        <v>-0.7760905300514792</v>
       </c>
       <c r="G100">
         <v>0</v>
@@ -3639,10 +3444,10 @@
         <v>-6.542064844563967</v>
       </c>
       <c r="E101">
-        <v>-6.943312027221621</v>
+        <v>-3.181569369598272</v>
       </c>
       <c r="F101">
-        <v>-5.726423479976549</v>
+        <v>-2.742191350691713</v>
       </c>
       <c r="G101">
         <v>0</v>
@@ -3671,10 +3476,10 @@
         <v>2.037058397194283</v>
       </c>
       <c r="E102">
-        <v>0.5503325671597774</v>
+        <v>-1.605609469145716</v>
       </c>
       <c r="F102">
-        <v>0.156537153976007</v>
+        <v>-0.7577406864233923</v>
       </c>
       <c r="G102">
         <v>0</v>
@@ -3703,10 +3508,10 @@
         <v>2.688045182252569</v>
       </c>
       <c r="E103">
-        <v>1.226075389186203</v>
+        <v>-1.119163756315846</v>
       </c>
       <c r="F103">
-        <v>1.42877232697495</v>
+        <v>0.5901045181152061</v>
       </c>
       <c r="G103">
         <v>0</v>
@@ -3735,10 +3540,10 @@
         <v>2.353950406955899</v>
       </c>
       <c r="E104">
-        <v>1.699292654879875</v>
+        <v>-0.02031902517221335</v>
       </c>
       <c r="F104">
-        <v>1.705033855971338</v>
+        <v>0.8726761879612995</v>
       </c>
       <c r="G104">
         <v>0</v>
@@ -3767,10 +3572,10 @@
         <v>0.3798511887855664</v>
       </c>
       <c r="E105">
-        <v>0.3772192015174867</v>
+        <v>0.07755790782150254</v>
       </c>
       <c r="F105">
-        <v>0.06472726619494605</v>
+        <v>-0.2336689889910659</v>
       </c>
       <c r="G105">
         <v>0.7491005630010378</v>
@@ -3799,10 +3604,10 @@
         <v>-1.318693536207314</v>
       </c>
       <c r="E106">
-        <v>-1.655452061583917</v>
+        <v>-1.158552660192015</v>
       </c>
       <c r="F106">
-        <v>-1.800529016720481</v>
+        <v>-1.397953852849606</v>
       </c>
       <c r="G106">
         <v>0.9661536508751972</v>
@@ -3831,10 +3636,10 @@
         <v>-1.132348538934526</v>
       </c>
       <c r="E107">
-        <v>-0.5028120675121113</v>
+        <v>0.4265273535101815</v>
       </c>
       <c r="F107">
-        <v>-0.8354087230988716</v>
+        <v>-0.6105857162344563</v>
       </c>
       <c r="G107">
         <v>0.9973888608694204</v>
@@ -3863,10 +3668,10 @@
         <v>0.02858416493522108</v>
       </c>
       <c r="E108">
-        <v>-0.2054536811164672</v>
+        <v>-0.4430172083825434</v>
       </c>
       <c r="F108">
-        <v>-0.4976640683771523</v>
+        <v>-0.6562543844156857</v>
       </c>
       <c r="G108">
         <v>0</v>
@@ -3895,10 +3700,10 @@
         <v>0.9797688071164382</v>
       </c>
       <c r="E109">
-        <v>0.678876920593153</v>
+        <v>-0.2076576129874506</v>
       </c>
       <c r="F109">
-        <v>0.1142093358590014</v>
+        <v>-0.5260817983063251</v>
       </c>
       <c r="G109">
         <v>1.340770335123714</v>
@@ -3927,10 +3732,10 @@
         <v>0.8076613064000865</v>
       </c>
       <c r="E110">
-        <v>0.2968929801286225</v>
+        <v>-0.6750220089667676</v>
       </c>
       <c r="F110">
-        <v>-0.4687446673920392</v>
+        <v>-1.148617932595298</v>
       </c>
       <c r="G110">
         <v>3.545424932912264</v>
@@ -3959,10 +3764,10 @@
         <v>-0.3411940348332417</v>
       </c>
       <c r="E111">
-        <v>0.3278024730586979</v>
+        <v>0.8117186944963267</v>
       </c>
       <c r="F111">
-        <v>-0.09650150433571714</v>
+        <v>-0.203668967250287</v>
       </c>
       <c r="G111">
         <v>1.701059743862671</v>
@@ -3991,10 +3796,10 @@
         <v>-0.4696901821878153</v>
       </c>
       <c r="E112">
-        <v>-0.47731295314911</v>
+        <v>-0.3853037634863717</v>
       </c>
       <c r="F112">
-        <v>-1.095337248574382</v>
+        <v>-1.247406360203464</v>
       </c>
       <c r="G112">
         <v>0</v>
@@ -4023,10 +3828,10 @@
         <v>-1.080390310211231</v>
       </c>
       <c r="E113">
-        <v>-0.3466060176204514</v>
+        <v>0.7519439241897261</v>
       </c>
       <c r="F113">
-        <v>-0.180580111238326</v>
+        <v>0.2828686702504825</v>
       </c>
       <c r="G113">
         <v>0</v>
@@ -4055,10 +3860,10 @@
         <v>-0.1842806384464342</v>
       </c>
       <c r="E114">
-        <v>0.06108286510110914</v>
+        <v>0.2673030181505062</v>
       </c>
       <c r="F114">
-        <v>-0.1111570037052949</v>
+        <v>-0.1378672765001468</v>
       </c>
       <c r="G114">
         <v>0</v>
@@ -4087,10 +3892,10 @@
         <v>-1.226991158476006</v>
       </c>
       <c r="E115">
-        <v>-1.416642096306022</v>
+        <v>-0.781476206733356</v>
       </c>
       <c r="F115">
-        <v>-1.191227095731085</v>
+        <v>-0.631374921740562</v>
       </c>
       <c r="G115">
         <v>0</v>
@@ -4119,10 +3924,10 @@
         <v>0.8998100472117867</v>
       </c>
       <c r="E116">
-        <v>0.8554870056926287</v>
+        <v>0.09860677958090081</v>
       </c>
       <c r="F116">
-        <v>0.02712488981398142</v>
+        <v>-0.7249180524238303</v>
       </c>
       <c r="G116">
         <v>0</v>
@@ -4151,10 +3956,10 @@
         <v>-1.291432823353359</v>
       </c>
       <c r="E117">
-        <v>-0.9777519962279194</v>
+        <v>-0.1933146340057839</v>
       </c>
       <c r="F117">
-        <v>-1.465963454515147</v>
+        <v>-1.260369574704796</v>
       </c>
       <c r="G117">
         <v>0</v>
@@ -4183,10 +3988,10 @@
         <v>0.2081233399037374</v>
       </c>
       <c r="E118">
-        <v>0.3560228454399778</v>
+        <v>0.3150243953774081</v>
       </c>
       <c r="F118">
-        <v>0.3042115030174405</v>
+        <v>0.2005762862393452</v>
       </c>
       <c r="G118">
         <v>0</v>
@@ -4215,10 +4020,10 @@
         <v>-1.172370348737002</v>
       </c>
       <c r="E119">
-        <v>-1.0502892368053</v>
+        <v>-0.3897819665195271</v>
       </c>
       <c r="F119">
-        <v>-1.318505639624381</v>
+        <v>-1.03877890171583</v>
       </c>
       <c r="G119">
         <v>0.1281076596132503</v>
@@ -4247,10 +4052,10 @@
         <v>0.2743287432270144</v>
       </c>
       <c r="E120">
-        <v>0.3983484310300183</v>
+        <v>0.2607426387189011</v>
       </c>
       <c r="F120">
-        <v>0.1807779061773665</v>
+        <v>-0.03228634811520034</v>
       </c>
       <c r="G120">
         <v>2.258379698976421</v>
@@ -4279,10 +4084,10 @@
         <v>-0.02903329557606984</v>
       </c>
       <c r="E121">
-        <v>-0.09791376062479359</v>
+        <v>-0.1159213378546167</v>
       </c>
       <c r="F121">
-        <v>-0.06989271093507674</v>
+        <v>-0.0439672711179927</v>
       </c>
       <c r="G121">
         <v>0</v>
@@ -4311,10 +4116,10 @@
         <v>-0.1087249927877601</v>
       </c>
       <c r="E122">
-        <v>-0.158767893129076</v>
+        <v>-0.3904304281756452</v>
       </c>
       <c r="F122">
-        <v>-1.127758829495763</v>
+        <v>-1.590853039841331</v>
       </c>
       <c r="G122">
         <v>0</v>
@@ -4343,10 +4148,10 @@
         <v>-0.1446867448648093</v>
       </c>
       <c r="E123">
-        <v>0.2670523912291083</v>
+        <v>0.6060888129928632</v>
       </c>
       <c r="F123">
-        <v>0.2936927299210498</v>
+        <v>0.3536350276378289</v>
       </c>
       <c r="G123">
         <v>0</v>
@@ -4375,10 +4180,10 @@
         <v>-0.8939912508170075</v>
       </c>
       <c r="E124">
-        <v>-0.5199160052039014</v>
+        <v>0.3222830315853672</v>
       </c>
       <c r="F124">
-        <v>-0.1054389798414038</v>
+        <v>0.4251142362929451</v>
       </c>
       <c r="G124">
         <v>0</v>
@@ -4407,10 +4212,10 @@
         <v>-1.995248174272763</v>
       </c>
       <c r="E125">
-        <v>-1.206533933378798</v>
+        <v>0.2639921899002131</v>
       </c>
       <c r="F125">
-        <v>-1.68905704124384</v>
+        <v>-1.234680103114009</v>
       </c>
       <c r="G125">
         <v>0</v>
@@ -4439,10 +4244,10 @@
         <v>-0.4235077844543399</v>
       </c>
       <c r="E126">
-        <v>-0.8334445374636075</v>
+        <v>-0.7840908115244252</v>
       </c>
       <c r="F126">
-        <v>-0.6089497446202558</v>
+        <v>-0.3347485307743378</v>
       </c>
       <c r="G126">
         <v>0</v>
@@ -4471,10 +4276,10 @@
         <v>0.8296762136516268</v>
       </c>
       <c r="E127">
-        <v>0.8086651034498265</v>
+        <v>0.2709381561770717</v>
       </c>
       <c r="F127">
-        <v>0.5918675026008394</v>
+        <v>0.1819979653708787</v>
       </c>
       <c r="G127">
         <v>0</v>
@@ -4503,10 +4308,10 @@
         <v>-0.3824041242321561</v>
       </c>
       <c r="E128">
-        <v>-0.7387032790243845</v>
+        <v>-0.7222319775432515</v>
       </c>
       <c r="F128">
-        <v>-0.6709008908369281</v>
+        <v>-0.4935084345214309</v>
       </c>
       <c r="G128">
         <v>0</v>
@@ -4535,10 +4340,10 @@
         <v>-0.6284075972838304</v>
       </c>
       <c r="E129">
-        <v>-0.03454112979517709</v>
+        <v>0.3983045090914834</v>
       </c>
       <c r="F129">
-        <v>-1.074873506631143</v>
+        <v>-1.397593415008195</v>
       </c>
       <c r="G129">
         <v>0</v>
@@ -4567,10 +4372,10 @@
         <v>-0.5824065415049382</v>
       </c>
       <c r="E130">
-        <v>-0.7727032071979599</v>
+        <v>-0.634223510873418</v>
       </c>
       <c r="F130">
-        <v>-1.042488470794282</v>
+        <v>-0.9708477638840224</v>
       </c>
       <c r="G130">
         <v>0</v>
@@ -4599,10 +4404,10 @@
         <v>1.02221679608991</v>
       </c>
       <c r="E131">
-        <v>0.942966941385064</v>
+        <v>0.1969932129369167</v>
       </c>
       <c r="F131">
-        <v>0.4874991961131585</v>
+        <v>-0.1144756077110131</v>
       </c>
       <c r="G131">
         <v>0</v>
@@ -4631,10 +4436,10 @@
         <v>-0.1909861387599138</v>
       </c>
       <c r="E132">
-        <v>-0.3004669069809409</v>
+        <v>-0.2564063783231639</v>
       </c>
       <c r="F132">
-        <v>-0.2881165369094977</v>
+        <v>-0.2116463549985411</v>
       </c>
       <c r="G132">
         <v>0</v>
@@ -4663,10 +4468,10 @@
         <v>0.3972132822498629</v>
       </c>
       <c r="E133">
-        <v>0.2581345931966431</v>
+        <v>-0.1304685082243044</v>
       </c>
       <c r="F133">
-        <v>-0.04019606018123319</v>
+        <v>-0.3355538902834415</v>
       </c>
       <c r="G133">
         <v>1.09803417378241</v>
@@ -4695,10 +4500,10 @@
         <v>-0.6692511236588188</v>
       </c>
       <c r="E134">
-        <v>-0.4981741429791404</v>
+        <v>-0.07878541494124258</v>
       </c>
       <c r="F134">
-        <v>-0.7227672568742248</v>
+        <v>-0.6016018064123865</v>
       </c>
       <c r="G134">
         <v>0.4669173513004787</v>
@@ -4727,10 +4532,10 @@
         <v>-0.6876298448841669</v>
       </c>
       <c r="E135">
-        <v>-0.3505434426495415</v>
+        <v>0.21773158336389</v>
       </c>
       <c r="F135">
-        <v>-0.4364170577366244</v>
+        <v>-0.2390117879133458</v>
       </c>
       <c r="G135">
         <v>0</v>
@@ -4759,10 +4564,10 @@
         <v>0.6513131116386077</v>
       </c>
       <c r="E136">
-        <v>0.3815628791822064</v>
+        <v>-0.2120028559323449</v>
       </c>
       <c r="F136">
-        <v>0.1472813588307929</v>
+        <v>-0.204168912315755</v>
       </c>
       <c r="G136">
         <v>0</v>
@@ -4791,10 +4596,10 @@
         <v>-0.3493016379398552</v>
       </c>
       <c r="E137">
-        <v>0.04888900594435236</v>
+        <v>0.3544723656041616</v>
       </c>
       <c r="F137">
-        <v>-0.4423590343466821</v>
+        <v>-0.5775454548817586</v>
       </c>
       <c r="G137">
         <v>1.468897904960685</v>
@@ -4823,10 +4628,10 @@
         <v>0.03851574765178775</v>
       </c>
       <c r="E138">
-        <v>-0.09763301516374037</v>
+        <v>-0.2732203739878872</v>
       </c>
       <c r="F138">
-        <v>-0.3602963498975854</v>
+        <v>-0.5084949783198731</v>
       </c>
       <c r="G138">
         <v>2.443610535370671</v>
@@ -4855,10 +4660,10 @@
         <v>-0.223604121537359</v>
       </c>
       <c r="E139">
-        <v>0.006088554836892607</v>
+        <v>0.2996600186797755</v>
       </c>
       <c r="F139">
-        <v>0.110112502790977</v>
+        <v>0.2410834614593476</v>
       </c>
       <c r="G139">
         <v>1.396959193747813</v>
@@ -4887,10 +4692,10 @@
         <v>-0.610616275133228</v>
       </c>
       <c r="E140">
-        <v>-0.3838153462780554</v>
+        <v>0.140357096720916</v>
       </c>
       <c r="F140">
-        <v>-0.2248586764076552</v>
+        <v>0.07350878993816971</v>
       </c>
       <c r="G140">
         <v>0.3618682483633031</v>
@@ -4919,10 +4724,10 @@
         <v>-0.5383687447975908</v>
       </c>
       <c r="E141">
-        <v>-0.582287470211573</v>
+        <v>-0.3256591941163419</v>
       </c>
       <c r="F141">
-        <v>-0.6532040790611651</v>
+        <v>-0.4962298746013376</v>
       </c>
       <c r="G141">
         <v>0</v>

</xml_diff>